<commit_message>
organizacion de archivos y carpetas
</commit_message>
<xml_diff>
--- a/MODELO DE FUGA/EarlyRetirementPrediction.xlsx
+++ b/MODELO DE FUGA/EarlyRetirementPrediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4e0323458c84468b/Hazel and Big Data/Business Intelligence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{0BC9E1A1-287F-48E3-870C-822BDB0BDA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB17357-0817-4EEE-A81B-F8C3B58DB6DD}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{0BC9E1A1-287F-48E3-870C-822BDB0BDA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD42CDB3-5FE8-4986-B6D4-DEB28DB58501}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BB7NV" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BB7NV!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BB7NV!$A$1:$M$1501</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -575,48 +575,48 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -931,7 +931,7 @@
   <dimension ref="A1:M1501"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -57993,7 +57993,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M1501" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -58167,6 +58167,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -58175,20 +58181,14 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29E20E65-8FB6-4B0C-8246-B5A83EB70714}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B722B94B-86CC-4C6B-A304-91D5396888CF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1F45E60-C0D5-44B3-96AC-419ABEC58BFC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F1FA465-EE67-4692-A98B-B22C75C77FAD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F1FA465-EE67-4692-A98B-B22C75C77FAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1F45E60-C0D5-44B3-96AC-419ABEC58BFC}"/>
 </file>
</xml_diff>